<commit_message>
removed delivery fees with auto import
</commit_message>
<xml_diff>
--- a/public/sample/order_sample.xlsx
+++ b/public/sample/order_sample.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Customer Name</t>
   </si>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>Total Amount</t>
-  </si>
-  <si>
-    <t>Delivery Fees</t>
   </si>
   <si>
     <t>Markup Delivery Fees</t>
@@ -411,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,16 +421,15 @@
     <col min="3" max="3" width="10" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" customWidth="1"/>
     <col min="7" max="7" width="18.140625" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" customWidth="1"/>
-    <col min="9" max="9" width="27.42578125" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="13.28515625" customWidth="1"/>
-    <col min="14" max="14" width="18.42578125" customWidth="1"/>
+    <col min="8" max="8" width="27.42578125" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" customWidth="1"/>
+    <col min="13" max="13" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -441,7 +437,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -464,55 +460,49 @@
       <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
+      <c r="L1" t="s">
+        <v>16</v>
       </c>
       <c r="M1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G2">
         <v>100000</v>
       </c>
-      <c r="H2">
-        <v>1000</v>
-      </c>
-      <c r="J2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>22</v>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
+        <v>17</v>
       </c>
       <c r="M2" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added pay later in order import
</commit_message>
<xml_diff>
--- a/public/sample/order_sample.xlsx
+++ b/public/sample/order_sample.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Customer Name</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>Extra Charges</t>
+  </si>
+  <si>
+    <t>Pay Later</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -411,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,7 +439,7 @@
     <col min="14" max="14" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -476,8 +482,11 @@
       <c r="N1" t="s">
         <v>18</v>
       </c>
+      <c r="O1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -516,6 +525,9 @@
       </c>
       <c r="N2" t="s">
         <v>19</v>
+      </c>
+      <c r="O2" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>